<commit_message>
lab 5 fully done
</commit_message>
<xml_diff>
--- a/lab5/comparison.xlsx
+++ b/lab5/comparison.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Method</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>F1</t>
+  </si>
+  <si>
+    <t>AUC</t>
   </si>
   <si>
     <t>RandomForestClassifier</t>
@@ -442,16 +445,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -467,117 +471,144 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4">
-        <v>0.8238456672991777</v>
+        <v>0.9070208728652751</v>
       </c>
       <c r="C2" s="4">
-        <v>0.8238456672991777</v>
+        <v>0.9070208728652751</v>
       </c>
       <c r="D2" s="4">
-        <v>0.8222149660913303</v>
+        <v>0.9064425894951549</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.993093831198981</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4">
-        <v>0.5075901328273245</v>
+        <v>0.5196078431372549</v>
       </c>
       <c r="C3" s="4">
-        <v>0.5075901328273245</v>
+        <v>0.5196078431372549</v>
       </c>
       <c r="D3" s="4">
-        <v>0.3737016973493162</v>
+        <v>0.3851106258813493</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.8676916925004734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>0.8159392789373814</v>
+        <v>0.857685009487666</v>
       </c>
       <c r="C4" s="4">
-        <v>0.8159392789373814</v>
+        <v>0.857685009487666</v>
       </c>
       <c r="D4" s="4">
-        <v>0.8217008039768197</v>
+        <v>0.8643479903394946</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.9627045973918885</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
-        <v>0.8810879190385832</v>
+        <v>0.9120809614168248</v>
       </c>
       <c r="C5" s="4">
-        <v>0.8810879190385832</v>
+        <v>0.9120809614168248</v>
       </c>
       <c r="D5" s="4">
-        <v>0.8797692952417386</v>
+        <v>0.911162618569057</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.9953297212902542</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4">
-        <v>0.8402909550917141</v>
+        <v>0.9117647058823529</v>
       </c>
       <c r="C6" s="4">
-        <v>0.8402909550917141</v>
+        <v>0.9117647058823529</v>
       </c>
       <c r="D6" s="4">
-        <v>0.838037746075916</v>
+        <v>0.9108786583476612</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.9943102371508604</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>0.849146110056926</v>
+        <v>0.8956356736242884</v>
       </c>
       <c r="C7" s="4">
-        <v>0.849146110056926</v>
+        <v>0.8956356736242884</v>
       </c>
       <c r="D7" s="4">
-        <v>0.856784769204948</v>
+        <v>0.8961795097186297</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.9871195519191381</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4">
-        <v>0.8089816571790006</v>
+        <v>0.8526249209361164</v>
       </c>
       <c r="C8" s="4">
-        <v>0.8089816571790006</v>
+        <v>0.8526249209361164</v>
       </c>
       <c r="D8" s="4">
-        <v>0.8040149430309623</v>
+        <v>0.8518567502077986</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.9841194560344118</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4">
-        <v>0.5578747628083491</v>
+        <v>0.3716002530044276</v>
       </c>
       <c r="C9" s="4">
-        <v>0.5578747628083491</v>
+        <v>0.3716002530044276</v>
       </c>
       <c r="D9" s="4">
-        <v>0.559759480617154</v>
+        <v>0.3399893085260272</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.6332914087797556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>